<commit_message>
the elements are inorder now
</commit_message>
<xml_diff>
--- a/Current/HTML elems/buttons.xlsx
+++ b/Current/HTML elems/buttons.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -424,14 +424,14 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>https://www.feimaoyun.com/</t>
+          <t>https://www.br.de/index.html</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>testing 5 / 5</t>
+          <t>testing 7 / 7</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
finished the changes for false positives
</commit_message>
<xml_diff>
--- a/Current/HTML elems/buttons.xlsx
+++ b/Current/HTML elems/buttons.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -424,14 +424,14 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>https://www.br.de/index.html</t>
+          <t>https://www.bidtheatre.com/</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>testing 7 / 7</t>
+          <t>chrome-extension://cjpalhdlnbpafiamejdnhcphjbkeiagm/document-blocked.html?details=%7B%22url%22%3A%22https%3A%2F%2Fwww.bidtheatre.com%2F%22%2C%22hn%22%3A%22www.bidtheatre.com%22%2C%22dn%22%3A%22bidtheatre.com%22%2C%22fs%22%3A%22%7C%7Cbidtheatre.com%5E%22%7D</t>
         </is>
       </c>
     </row>

</xml_diff>